<commit_message>
Fully implement new spreadsheet system
</commit_message>
<xml_diff>
--- a/data/trivia_questions.xlsx
+++ b/data/trivia_questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\Projects\Python\EngineeringBot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{711D3C6E-24F2-4038-A44E-2190300101AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA8BC58-AC8D-47C2-944A-D99B6E8CC881}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
   <si>
     <t>category</t>
   </si>
@@ -40,32 +40,94 @@
     <t>structures</t>
   </si>
   <si>
-    <t>Cool;;Answer;;Bro</t>
-  </si>
-  <si>
-    <t>this is the answer message, haha</t>
-  </si>
-  <si>
-    <t>testing, this, thing?
-This question has multiple lines κκκκ ooo</t>
-  </si>
-  <si>
     <t>materials</t>
   </si>
   <si>
-    <t>next question</t>
-  </si>
-  <si>
-    <t>Answers;;Are;;Cool</t>
-  </si>
-  <si>
-    <t>very nice friend</t>
-  </si>
-  <si>
     <t>question_text</t>
   </si>
   <si>
     <t>sc_reward</t>
+  </si>
+  <si>
+    <t>Part 1A Materials Handout 4: Microstructure and Properties</t>
+  </si>
+  <si>
+    <t>G = elastic shear modulus, b = Burgers vector (atomic spacing), L = obstacle spacing, α = obstacle strength</t>
+  </si>
+  <si>
+    <t>maths</t>
+  </si>
+  <si>
+    <t>What is the convergence of a fourier series of a function with a discontinuity in gradient (first derivative)?</t>
+  </si>
+  <si>
+    <t>Part 1A Lent Term Mathematics</t>
+  </si>
+  <si>
+    <t>What is the convergence of a fourier series of a function with a discontinuity in the second derivative?</t>
+  </si>
+  <si>
+    <t>What is the convergence of a fourier series of a function with a discontinuity in the value?</t>
+  </si>
+  <si>
+    <t>What is the convergence of a fourier series of a function which is a series of delta functions?</t>
+  </si>
+  <si>
+    <t>When you transform wood (with modulus `E_w`) into steel (with modulus `E_s`) for analysis of composite beams made up of wood and steel, what happens to the width of the transformed section of wood?</t>
+  </si>
+  <si>
+    <t>Part 1A Structures Handout 6: Stresses Elastic Beams</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We take the bending stiffness `B=EI` to be constant for both wood and steel, where `I = (b*d^3)/12` for rectangular sections. By rearranging `E_w*I_w = E_s*I_s` you can find that the width of wood, for which `E_w&lt;E_s` is reduced by a factor of `E_w/E_s` when transformed into steel. </t>
+  </si>
+  <si>
+    <t>Which of the below statements are correct?</t>
+  </si>
+  <si>
+    <t>A light, simply supported beam is subject to a point load at its centre, of magnitude `p`. What is the minimum shear force in the beam?</t>
+  </si>
+  <si>
+    <t>simply_supported_beam_0.png</t>
+  </si>
+  <si>
+    <t>2009 1A P2 Q5</t>
+  </si>
+  <si>
+    <t>The contribution to the yield stress due to **dislocation pinning** depends directly on G, b, L, and α.
+Which of these properties can be manipulated by composition and processing and which are fixed parameters?</t>
+  </si>
+  <si>
+    <t>1/(n^2);;1/(n^3);;1/n;;Does not converge</t>
+  </si>
+  <si>
+    <t>1/(n^3);;1/(n^2);;1/n;;Does not converge</t>
+  </si>
+  <si>
+    <t>1/n;;1/(n^3);;1/(n^2);;Does not converge</t>
+  </si>
+  <si>
+    <t>Does not converge;;1/n;;1/(n^3);;1/(n^2)</t>
+  </si>
+  <si>
+    <t>`κ = -d²v/dx²`;;`∫v dx = -κ`;;`dκ/dx = M`;;`κ = -dΨ/dx`</t>
+  </si>
+  <si>
+    <t>`-p/2`;;`0`;;`p`;;`-p²`;;`-2p`;;`-p`</t>
+  </si>
+  <si>
+    <t>L and α can be manipulated, b and G are fixed.
+L and b can be manipulated, G and α are fixed.
+G and α can be manipulated, L and b are fixed.
+L and G can be manipulated, b and α are fixed.
+G and b can be manipulated, L and α are fixed.</t>
+  </si>
+  <si>
+    <t>Gets shorter by a factor of `E_w/E_s`
+Doesn't change
+Gets wider by a factor of `E_s/E_w`
+Gets shorter by a factor of `E_s`
+Gets shorter by a factor of `E_w`</t>
   </si>
 </sst>
 </file>
@@ -912,16 +974,18 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
-    <col min="3" max="3" width="49.42578125" customWidth="1"/>
-    <col min="4" max="6" width="24.85546875" customWidth="1"/>
-    <col min="7" max="7" width="46.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" customWidth="1"/>
+    <col min="4" max="4" width="61" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" customWidth="1"/>
+    <col min="6" max="6" width="47.7109375" customWidth="1"/>
+    <col min="7" max="7" width="63.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -929,16 +993,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
         <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -947,96 +1011,160 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1">
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="B4" s="1">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="F5" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="F6" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+    <row r="7" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>10</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="F7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1">
+        <v>4</v>
+      </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="F8" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1">
+        <v>6</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1113,6 +1241,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Pushed my version of trivia_questions
</commit_message>
<xml_diff>
--- a/data/trivia_questions.xlsx
+++ b/data/trivia_questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\Projects\Python\EngineeringBot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC8FAFA0-D85C-48E1-AB9C-5A931D7DDD4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3363F58A-B341-45F4-B823-BE177768DB9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -989,7 +989,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add is_multiple_choice to trivia questions
</commit_message>
<xml_diff>
--- a/data/trivia_questions.xlsx
+++ b/data/trivia_questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\Projects\Python\EngineeringBot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3363F58A-B341-45F4-B823-BE177768DB9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF34937-864D-405B-8FAE-5411E3429BC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
   <si>
     <t>category</t>
   </si>
@@ -143,6 +143,12 @@
   </si>
   <si>
     <t>**Isochoric** means **volume** is constant, **isothermal** means **temperature** is constant, and **isobaric** means **pressure** is constant.</t>
+  </si>
+  <si>
+    <t>is_multiple_choice</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -986,10 +992,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -999,11 +1005,13 @@
     <col min="3" max="3" width="28.5703125" customWidth="1"/>
     <col min="4" max="4" width="61" customWidth="1"/>
     <col min="5" max="5" width="28.5703125" customWidth="1"/>
-    <col min="6" max="6" width="47.7109375" customWidth="1"/>
-    <col min="7" max="7" width="63.5703125" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1"/>
+    <col min="7" max="7" width="47.7109375" customWidth="1"/>
+    <col min="8" max="8" width="63.5703125" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1020,13 +1028,16 @@
         <v>1</v>
       </c>
       <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1041,13 +1052,16 @@
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -1062,11 +1076,14 @@
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -1081,11 +1098,14 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -1100,11 +1120,14 @@
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -1119,11 +1142,14 @@
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1138,13 +1164,16 @@
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -1157,11 +1186,14 @@
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1178,11 +1210,14 @@
         <v>22</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>34</v>
       </c>
@@ -1197,13 +1232,16 @@
         <v>33</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1211,8 +1249,9 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1220,8 +1259,9 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1229,8 +1269,9 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1238,8 +1279,9 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1247,8 +1289,9 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1256,8 +1299,9 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1265,6 +1309,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fully implement "standard" question system
</commit_message>
<xml_diff>
--- a/data/trivia_questions.xlsx
+++ b/data/trivia_questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\Projects\Python\EngineeringBot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF34937-864D-405B-8FAE-5411E3429BC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45EA554-A4F0-4E2A-916C-1B792B9E0C25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -994,8 +994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>